<commit_message>
changes to flowchart of pregnancies
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY_COHORT.xlsx
+++ b/i_codebooks/D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY_COHORT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\DP3-MS-SLE\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lol\Documents\DP3-MS-SLE\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4719389-78E0-448D-8F56-3EA3337C0286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
     <sheet name="Parameters" sheetId="3" r:id="rId3"/>
     <sheet name="Example" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mhzNGBeK9861EYEtgLjD+CXFeX/VQ=="/>
@@ -246,9 +247,6 @@
     <t>EXCLUSION_2_pregnancy_not_in_fertile_age</t>
   </si>
   <si>
-    <t>DU_pregnancy_study_end_date &lt; 50th birthday &amp; DU_pregnancy_study_entry_date &gt;= 15th birthday</t>
-  </si>
-  <si>
     <t xml:space="preserve">DAP-specific
 for UOSL: ((type_of_end == "LB" OR type_of_end == "SB") AND PROMPT == "yes") OR (type_of_end == "SA" OR type_of_end == "T")
 for THL: …
@@ -264,16 +262,26 @@
   <si>
     <t>EXCLUSION_4_pregnancy_outside_period_with_medicines</t>
   </si>
+  <si>
+    <t>DU_pregnancy_study_end_date &lt; 50th birthday &amp; DU_pregnancy_study_entry_date &gt;= 15th birthday (0 if rule is true)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -568,133 +576,136 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -906,14 +917,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41.44140625" customWidth="1"/>
     <col min="2" max="2" width="75.21875" style="13" customWidth="1"/>
@@ -9389,19 +9400,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="38.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.88671875" customWidth="1"/>
     <col min="2" max="2" width="82.44140625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
@@ -9446,7 +9457,7 @@
       <c r="J1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="44" t="s">
         <v>22</v>
       </c>
     </row>
@@ -9617,7 +9628,7 @@
       <c r="I11" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="K11" s="47" t="s">
         <v>54</v>
       </c>
     </row>
@@ -9636,7 +9647,7 @@
       <c r="I12" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="47" t="s">
         <v>56</v>
       </c>
     </row>
@@ -9645,7 +9656,7 @@
         <v>69</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>59</v>
@@ -9657,8 +9668,8 @@
       <c r="I13" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="44" t="s">
-        <v>72</v>
+      <c r="K13" s="48" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="58.8" customHeight="1">
@@ -9678,8 +9689,8 @@
       <c r="I14" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="46" t="s">
-        <v>71</v>
+      <c r="K14" s="49" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="28.2" customHeight="1">
@@ -9701,13 +9712,13 @@
       <c r="I15" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="47" t="s">
+      <c r="K15" s="45" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="51.6" customHeight="1">
       <c r="A16" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>66</v>
@@ -9721,8 +9732,8 @@
       <c r="I16" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="48" t="s">
-        <v>73</v>
+      <c r="K16" s="46" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -10710,14 +10721,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10.6640625" customWidth="1"/>
   </cols>
@@ -11745,14 +11756,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10.6640625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
added exclusion criterion for non-female pregnant persons
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY_COHORT.xlsx
+++ b/i_codebooks/D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY_COHORT.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lol\Documents\DP3-MS-SLE\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\DP3-MS-SLE\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4719389-78E0-448D-8F56-3EA3337C0286}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8784" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
   <si>
     <t>medatata_name</t>
   </si>
@@ -238,15 +237,6 @@
     <t>This binary variable excludes those pregnancies if the pregnant person is younger than 15 or older than 49 during between pregnancy end and pregnancy</t>
   </si>
   <si>
-    <t>EXCLUSION_3_pregnancy_not_in_study_period</t>
-  </si>
-  <si>
-    <t>EXCLUSION_1_pregnancy_with_inappropriate_quality</t>
-  </si>
-  <si>
-    <t>EXCLUSION_2_pregnancy_not_in_fertile_age</t>
-  </si>
-  <si>
     <t xml:space="preserve">DAP-specific
 for UOSL: ((type_of_end == "LB" OR type_of_end == "SB") AND PROMPT == "yes") OR (type_of_end == "SA" OR type_of_end == "T")
 for THL: …
@@ -260,21 +250,46 @@
     <t>This is a variable created by each DAP. It excludes from the output of the ConcePTION Pregnancy Algorithm those pregnancies that are not considered to be appripriate for inclusion in the study</t>
   </si>
   <si>
-    <t>EXCLUSION_4_pregnancy_outside_period_with_medicines</t>
+    <t>DU_pregnancy_study_end_date &lt; 50th birthday &amp; DU_pregnancy_study_entry_date &gt;= 15th birthday (0 if rule is true)</t>
   </si>
   <si>
-    <t>DU_pregnancy_study_end_date &lt; 50th birthday &amp; DU_pregnancy_study_entry_date &gt;= 15th birthday (0 if rule is true)</t>
+    <t>EXCLUSION_2_pregnancy_with_inappropriate_quality</t>
+  </si>
+  <si>
+    <t>EXCLUSION_3_pregnancy_not_in_fertile_age</t>
+  </si>
+  <si>
+    <t>EXCLUSION_4_pregnancy_not_in_study_period</t>
+  </si>
+  <si>
+    <t>EXCLUSION_5_pregnancy_outside_period_with_medicines</t>
+  </si>
+  <si>
+    <t>sex_at_instance_creation != "F"</t>
+  </si>
+  <si>
+    <t>EXCLUSION_1_pregnancy_in_persons_of_non_female_gender</t>
+  </si>
+  <si>
+    <t>Excludes pregnancies whose pregnanct person is not declared female at the moment when the instance was created</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -576,136 +591,140 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -917,14 +936,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41.44140625" customWidth="1"/>
     <col min="2" max="2" width="75.21875" style="13" customWidth="1"/>
@@ -9400,17 +9419,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K994"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K995"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A13" sqref="A13:XFD13"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41.88671875" customWidth="1"/>
     <col min="2" max="2" width="82.44140625" style="13" bestFit="1" customWidth="1"/>
@@ -9651,12 +9670,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="42" customHeight="1">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1">
       <c r="A13" s="40" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C13" s="40" t="s">
         <v>59</v>
@@ -9665,19 +9684,19 @@
         <v>60</v>
       </c>
       <c r="E13" s="42"/>
-      <c r="I13" s="26" t="s">
+      <c r="I13" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="48" t="s">
-        <v>71</v>
+      <c r="K13" s="51" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="58.8" customHeight="1">
+    <row r="14" spans="1:11" ht="42" customHeight="1">
       <c r="A14" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>70</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>67</v>
       </c>
       <c r="C14" s="40" t="s">
         <v>59</v>
@@ -9689,16 +9708,16 @@
       <c r="I14" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="28.2" customHeight="1">
-      <c r="A15" s="40" t="s">
+      <c r="K14" s="48" t="s">
         <v>68</v>
       </c>
+    </row>
+    <row r="15" spans="1:11" ht="58.8" customHeight="1">
+      <c r="A15" s="40" t="s">
+        <v>73</v>
+      </c>
       <c r="B15" s="13" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C15" s="40" t="s">
         <v>59</v>
@@ -9706,22 +9725,20 @@
       <c r="D15" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="E15" s="42"/>
+      <c r="I15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="K15" s="45" t="s">
-        <v>61</v>
+      <c r="K15" s="49" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="51.6" customHeight="1">
+    <row r="16" spans="1:11" ht="28.2" customHeight="1">
       <c r="A16" s="40" t="s">
         <v>74</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C16" s="40" t="s">
         <v>59</v>
@@ -9729,29 +9746,51 @@
       <c r="D16" s="13" t="s">
         <v>60</v>
       </c>
+      <c r="E16" s="13" t="s">
+        <v>65</v>
+      </c>
       <c r="I16" t="s">
         <v>30</v>
       </c>
-      <c r="K16" s="46" t="s">
-        <v>72</v>
+      <c r="K16" s="45" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:11" ht="51.6" customHeight="1">
+      <c r="A17" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" s="46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:11" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:11" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -10714,6 +10753,7 @@
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10721,14 +10761,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10.6640625" customWidth="1"/>
   </cols>
@@ -11756,14 +11796,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="26" width="10.6640625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Updated codebooks for period non pregnant
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY_COHORT.xlsx
+++ b/i_codebooks/D3_DU_selection_criteria_from_pregnancies_to_DU_PREGNANCY_COHORT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE - Copy\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0B38FE-4969-41CE-AD97-51A0AEC3C599}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54006068-1001-4C5B-A5B0-09379F637BA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -940,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -9423,16 +9423,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K995"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A2:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="69.7109375" customWidth="1"/>
     <col min="2" max="2" width="82.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>

</xml_diff>